<commit_message>
Uploaded 06-Aug-2021 10:15:49 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -54,28 +54,28 @@
     <t xml:space="preserve">Loan from $loan</t>
   </si>
   <si>
+    <t xml:space="preserve">$address: mailingAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$loan: loan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annualIncome &gt;= $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyDebt &lt;= $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type == "$param"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount &gt; $param</t>
+  </si>
+  <si>
     <t xml:space="preserve">Address(state in ($param)) from $address</t>
   </si>
   <si>
     <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$address: mailingAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$loan: loan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annualIncome &gt;= $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyDebt &lt;= $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type == "$param"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount &gt; $param</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Income</t>
@@ -228,8 +228,8 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -240,8 +240,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="35.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="39.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,30 +302,30 @@
         <v>9</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="I7" s="0" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:18:14 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t xml:space="preserve">Ruleset</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule Name</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Income</t>
@@ -228,8 +231,8 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -330,34 +333,37 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>5000</v>
@@ -366,16 +372,16 @@
         <v>200</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>30000</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:18:57 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -39,6 +39,9 @@
     <t xml:space="preserve">RuleTable</t>
   </si>
   <si>
+    <t xml:space="preserve">Rule Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONDITON</t>
   </si>
   <si>
@@ -76,9 +79,6 @@
   </si>
   <si>
     <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule Name</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Income</t>
@@ -232,7 +232,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,73 +269,73 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:19:49 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t xml:space="preserve">Ruleset</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Rule 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">Mortgage</t>
@@ -232,7 +229,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,12 +356,6 @@
       <c r="A9" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="D9" s="0" t="n">
         <v>5000</v>
       </c>
@@ -372,16 +363,16 @@
         <v>200</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>30000</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:22:20 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t xml:space="preserve">Ruleset</t>
   </si>
@@ -31,9 +31,9 @@
     <t xml:space="preserve">import</t>
   </si>
   <si>
-    <t xml:space="preserve">import com.blackknight.demo.models.MortgageRequest;
-import com.blackknight.demo.models.Address;
-import com.blackknight.demo.models.Loan;</t>
+    <t xml:space="preserve">com.blackknight.demo.models.MortgageRequest;
+com.blackknight.demo.models.Address;
+Com.blackknight.demo.models.Loan;</t>
   </si>
   <si>
     <t xml:space="preserve">RuleTable</t>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rule 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">Mortgage</t>
@@ -229,7 +232,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -356,6 +359,12 @@
       <c r="A9" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" s="0" t="n">
         <v>5000</v>
       </c>
@@ -363,16 +372,16 @@
         <v>200</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>30000</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:25:25 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve">Ruleset</t>
   </si>
@@ -31,9 +31,9 @@
     <t xml:space="preserve">import</t>
   </si>
   <si>
-    <t xml:space="preserve">com.blackknight.demo.models.MortgageRequest;
-com.blackknight.demo.models.Address;
-Com.blackknight.demo.models.Loan;</t>
+    <t xml:space="preserve">com.blackknight.demo.models.MortgageRequest,
+com.blackknight.demo.models.Address,
+Com.blackknight.demo.models.Loan</t>
   </si>
   <si>
     <t xml:space="preserve">RuleTable</t>
@@ -57,13 +57,7 @@
     <t xml:space="preserve">Loan from $loan</t>
   </si>
   <si>
-    <t xml:space="preserve">$address: mailingAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$loan: loan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annualIncome &gt;= $param</t>
+    <t xml:space="preserve">$address: mailingAddress,$loan: loan,annualIncome &gt;= $param</t>
   </si>
   <si>
     <t xml:space="preserve">monthlyDebt &lt;= $param</t>
@@ -100,9 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">Rule 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">Mortgage</t>
@@ -229,22 +220,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="41.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="39.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,19 +270,13 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -302,12 +285,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
@@ -328,14 +309,14 @@
       <c r="G7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
@@ -348,46 +329,34 @@
       <c r="G8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>30000</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:26:01 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -39,7 +39,7 @@
     <t xml:space="preserve">RuleTable</t>
   </si>
   <si>
-    <t xml:space="preserve">Rule Name</t>
+    <t xml:space="preserve">RuleName</t>
   </si>
   <si>
     <t xml:space="preserve">CONDITON</t>
@@ -223,7 +223,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:29:17 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t xml:space="preserve">Ruleset</t>
   </si>
@@ -39,42 +39,42 @@
     <t xml:space="preserve">RuleTable</t>
   </si>
   <si>
+    <t xml:space="preserve">CONDITON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONDITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$application : MortgageRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loan from $loan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$address: mailingAddress,$loan: loan,annualIncome &gt;= $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyDebt &lt;= $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type == "$param"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount &gt; $param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address(state in ($param)) from $address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
+  </si>
+  <si>
     <t xml:space="preserve">RuleName</t>
   </si>
   <si>
-    <t xml:space="preserve">CONDITON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONDITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$application : MortgageRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loan from $loan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$address: mailingAddress,$loan: loan,annualIncome &gt;= $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyDebt &lt;= $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type == "$param"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount &gt; $param</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address(state in ($param)) from $address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
-  </si>
-  <si>
     <t xml:space="preserve">Annual Income</t>
   </si>
   <si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t xml:space="preserve">Approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“NY”,”CA”,”TN”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denied</t>
   </si>
 </sst>
 </file>
@@ -220,10 +229,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -234,6 +243,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,110 +263,133 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>5000</v>
-      </c>
       <c r="C9" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>30000</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:31:54 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -32,8 +32,7 @@
   </si>
   <si>
     <t xml:space="preserve">com.blackknight.demo.models.MortgageRequest,
-com.blackknight.demo.models.Address,
-Com.blackknight.demo.models.Loan</t>
+com.blackknight.demo.models.Address,com.blackknight.demo.models.Loan</t>
   </si>
   <si>
     <t xml:space="preserve">RuleTable</t>
@@ -191,17 +190,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -231,14 +226,14 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.1"/>
@@ -254,7 +249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="33.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="22.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -271,16 +266,16 @@
       <c r="C5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -288,14 +283,14 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
@@ -321,22 +316,22 @@
       <c r="B8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:38:18 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
   </si>
   <si>
-    <t xml:space="preserve">RuleName</t>
+    <t xml:space="preserve">Rule Name</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Income</t>
@@ -120,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -147,13 +147,56 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1C1C1C"/>
+        <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF860D"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF50938A"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,20 +233,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,6 +279,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF2A6099"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF860D"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF50938A"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF1C1C1C"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -227,12 +350,12 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.5"/>
@@ -242,18 +365,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="22.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -263,34 +386,34 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
@@ -313,25 +436,25 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="8" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:39:43 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -38,6 +38,9 @@
     <t xml:space="preserve">RuleTable</t>
   </si>
   <si>
+    <t xml:space="preserve">NAME</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONDITON</t>
   </si>
   <si>
@@ -69,9 +72,6 @@
   </si>
   <si>
     <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule Name</t>
   </si>
   <si>
     <t xml:space="preserve">Annual Income</t>
@@ -120,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,6 +144,12 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -233,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,11 +256,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,11 +272,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,7 +360,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -386,75 +396,76 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="H5" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="9" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:41:34 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -272,7 +272,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,7 +360,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,7 +391,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:45:56 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -25,14 +25,15 @@
     <t xml:space="preserve">Ruleset</t>
   </si>
   <si>
-    <t xml:space="preserve">com.blackknight.demo.rules</t>
+    <t xml:space="preserve">com.blackknightdemo.dmnrulesdemo</t>
   </si>
   <si>
     <t xml:space="preserve">import</t>
   </si>
   <si>
     <t xml:space="preserve">com.blackknight.demo.models.MortgageRequest,
-com.blackknight.demo.models.Address,com.blackknight.demo.models.Loan</t>
+com.blackknight.demo.models.Address,
+com.blackknight.demo.models.Loan</t>
   </si>
   <si>
     <t xml:space="preserve">RuleTable</t>
@@ -56,7 +57,7 @@
     <t xml:space="preserve">Loan from $loan</t>
   </si>
   <si>
-    <t xml:space="preserve">$address: mailingAddress,$loan: loan,annualIncome &gt;= $param</t>
+    <t xml:space="preserve">$address: mailingAddress,$loan: loan,annualIncome &lt;= $param</t>
   </si>
   <si>
     <t xml:space="preserve">monthlyDebt &lt;= $param</t>
@@ -148,6 +149,13 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -159,15 +167,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +183,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFD4EA6B"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF1C1C1C"/>
       </patternFill>
     </fill>
     <fill>
@@ -200,12 +207,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF2A6099"/>
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -213,6 +226,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -239,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,27 +276,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,11 +354,11 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFD4EA6B"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -357,16 +385,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.1"/>
@@ -382,7 +410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="22.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="33.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -391,134 +419,134 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="11" t="n">
         <v>50000</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="C9" s="11" t="n">
         <v>200</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="E9" s="11" t="n">
         <v>30000</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="F9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="G9" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="B10" s="11" t="n">
         <v>70000</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="C10" s="11" t="n">
         <v>400</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="E10" s="11" t="n">
         <v>20000</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="F10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="G10" s="11" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 10:49:29 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t xml:space="preserve">Ruleset</t>
   </si>
@@ -57,6 +57,9 @@
     <t xml:space="preserve">Loan from $loan</t>
   </si>
   <si>
+    <t xml:space="preserve">Address from $address</t>
+  </si>
+  <si>
     <t xml:space="preserve">$address: mailingAddress,$loan: loan,annualIncome &lt;= $param</t>
   </si>
   <si>
@@ -69,7 +72,7 @@
     <t xml:space="preserve">Amount &gt; $param</t>
   </si>
   <si>
-    <t xml:space="preserve">Address(state in ($param)) from $address</t>
+    <t xml:space="preserve">state in ($param)</t>
   </si>
   <si>
     <t xml:space="preserve">modify($application) { setStatus("$param")};</t>
@@ -259,7 +262,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,6 +297,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -388,7 +395,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -455,92 +462,95 @@
         <v>10</v>
       </c>
       <c r="E6" s="8"/>
+      <c r="F6" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>22</v>
       </c>
+      <c r="G8" s="11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="11" t="n">
+      <c r="A9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="12" t="n">
         <v>50000</v>
       </c>
-      <c r="C9" s="11" t="n">
+      <c r="C9" s="12" t="n">
         <v>200</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="11" t="n">
+      <c r="D9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="12" t="n">
         <v>30000</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="12" t="n">
+        <v>70000</v>
+      </c>
+      <c r="C10" s="12" t="n">
+        <v>400</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="11" t="n">
-        <v>70000</v>
-      </c>
-      <c r="C10" s="11" t="n">
-        <v>400</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="11" t="n">
+      <c r="E10" s="12" t="n">
         <v>20000</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="11" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 06-Aug-2021 11:04:37 {/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
+++ b/src/main/resources/com/blackknightdemo/dmnrulesdemo/TestRules.xlsx
@@ -60,7 +60,7 @@
     <t>type == "$param"</t>
   </si>
   <si>
-    <t>Amount &gt; $param</t>
+    <t>amount &gt; $param</t>
   </si>
   <si>
     <t>state in ($param)</t>
@@ -112,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -138,6 +138,9 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -242,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -275,6 +278,9 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -284,7 +290,7 @@
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -581,7 +587,7 @@
       <c r="D7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="11" t="s">
@@ -592,69 +598,69 @@
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="15">
         <v>50000.0</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="15">
         <v>200.0</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="15">
         <v>30000.0</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="15">
         <v>70000.0</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="15">
         <v>400.0</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="15">
         <v>20000.0</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="15" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>